<commit_message>
final version of controller
</commit_message>
<xml_diff>
--- a/Résultats controller PI.xlsx
+++ b/Résultats controller PI.xlsx
@@ -181,6 +181,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -190,7 +191,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -495,7 +495,7 @@
   <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -638,13 +638,13 @@
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="8"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
@@ -695,13 +695,13 @@
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="8"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
@@ -839,7 +839,7 @@
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
-      <c r="E27" s="8" t="s">
+      <c r="E27" s="5" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>